<commit_message>
Split Point Detail Excel
</commit_message>
<xml_diff>
--- a/matlab/SplitPointLocaiton_Details.xlsx
+++ b/matlab/SplitPointLocaiton_Details.xlsx
@@ -7729,8 +7729,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="D61" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>